<commit_message>
Analisis de requerimientos sobre servicios SOA y especificacion de requerimientos asociados
</commit_message>
<xml_diff>
--- a/Analisis/Portafolio_Servicios_SOA.xlsx
+++ b/Analisis/Portafolio_Servicios_SOA.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="PORTAFOLIO_SERVICIOS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="179">
   <si>
     <t>ID</t>
   </si>
@@ -308,6 +308,249 @@
   </si>
   <si>
     <t>faultOperation</t>
+  </si>
+  <si>
+    <t>CAPACIDAD</t>
+  </si>
+  <si>
+    <t>Añadir adjuntos</t>
+  </si>
+  <si>
+    <t>Añadir comentario</t>
+  </si>
+  <si>
+    <t>Reclamar la tarea</t>
+  </si>
+  <si>
+    <t>Realizar reclamo de tarea en lote</t>
+  </si>
+  <si>
+    <t>Marcar tarea completada</t>
+  </si>
+  <si>
+    <t>Marcar tarea completada en lote</t>
+  </si>
+  <si>
+    <t>Delegar la tarea</t>
+  </si>
+  <si>
+    <t>Delegar la tarea en lote</t>
+  </si>
+  <si>
+    <t>Eliminar adjunto</t>
+  </si>
+  <si>
+    <t>Eliminar comentario</t>
+  </si>
+  <si>
+    <t>Eliminar falla</t>
+  </si>
+  <si>
+    <t>Fallar la tarea</t>
+  </si>
+  <si>
+    <t>Fallar tareas en lote</t>
+  </si>
+  <si>
+    <t>Mover tarea adelante</t>
+  </si>
+  <si>
+    <t>Mover tarea adelante en lote</t>
+  </si>
+  <si>
+    <t>Obtener adjunto</t>
+  </si>
+  <si>
+    <t>Obtener información de adjuntos</t>
+  </si>
+  <si>
+    <t>Obtener comentarios</t>
+  </si>
+  <si>
+    <t>Obtener falla de tarea</t>
+  </si>
+  <si>
+    <t>Obtener información de entrada a la tarea</t>
+  </si>
+  <si>
+    <t>Eliminar salida de la tarea</t>
+  </si>
+  <si>
+    <t>Obtener salida de la tarea</t>
+  </si>
+  <si>
+    <t>Obtener resultado de accion de finalización de la tarea</t>
+  </si>
+  <si>
+    <t>Obtener la tarea padre</t>
+  </si>
+  <si>
+    <t>Obtener Identificador de la tarea padre</t>
+  </si>
+  <si>
+    <t>Obtener visualización de la tarea</t>
+  </si>
+  <si>
+    <t>Obtener tipos de visualizaciones</t>
+  </si>
+  <si>
+    <t>Obtener identificadores de la tarea</t>
+  </si>
+  <si>
+    <t>Obtener Subtareas</t>
+  </si>
+  <si>
+    <t>Obtener Descripcion de la tarea</t>
+  </si>
+  <si>
+    <t>Obtener detalles de la tarea</t>
+  </si>
+  <si>
+    <t>Obtener historia de la tarea</t>
+  </si>
+  <si>
+    <t>Obteher Datos de Instancia de la Tarea</t>
+  </si>
+  <si>
+    <t>Obtener las operaciones de la tarea</t>
+  </si>
+  <si>
+    <t>Determinar si tiene subtareas</t>
+  </si>
+  <si>
+    <t>Instanciar subtarea</t>
+  </si>
+  <si>
+    <t>Determinar si es una subtarea</t>
+  </si>
+  <si>
+    <t>Liberar la tarea</t>
+  </si>
+  <si>
+    <t>Liberar tareas en lote</t>
+  </si>
+  <si>
+    <t>Remover tarea</t>
+  </si>
+  <si>
+    <t>Remiver tarea en lote</t>
+  </si>
+  <si>
+    <t>Re-iniciar la tarea</t>
+  </si>
+  <si>
+    <t>Re-iniciar tareas en lote</t>
+  </si>
+  <si>
+    <t>Establecer falla de la tarea</t>
+  </si>
+  <si>
+    <t>Establecer la salida de la tarea</t>
+  </si>
+  <si>
+    <t>Establecer la prioridad</t>
+  </si>
+  <si>
+    <t>Establecer prioridad en lote</t>
+  </si>
+  <si>
+    <t>Establecer Expresion de fecha limite de completamiento</t>
+  </si>
+  <si>
+    <t>Establecer Expresion de fecha limite de duracion</t>
+  </si>
+  <si>
+    <t>Establecer Expresión de fecha limite para inicio de tarea</t>
+  </si>
+  <si>
+    <t>Establecer expresion de duración de inicio de tarea</t>
+  </si>
+  <si>
+    <t>Saltar la tarea</t>
+  </si>
+  <si>
+    <t>Saltar tareas en lote</t>
+  </si>
+  <si>
+    <t>Iniciar la tarea</t>
+  </si>
+  <si>
+    <t>Iniciar tareas en lote</t>
+  </si>
+  <si>
+    <t>Detener tarea</t>
+  </si>
+  <si>
+    <t>Detener tareas en lote</t>
+  </si>
+  <si>
+    <t>Suspender la tarea</t>
+  </si>
+  <si>
+    <t>Suspender tareas en lote</t>
+  </si>
+  <si>
+    <t>Suspender tarea hasta condicion</t>
+  </si>
+  <si>
+    <t>Suspender tareas en lote hasta condicion</t>
+  </si>
+  <si>
+    <t>Actualizar comentario</t>
+  </si>
+  <si>
+    <t>Obtener información abstracta de mi tarea</t>
+  </si>
+  <si>
+    <t>Obtener información detallada de mi tarea</t>
+  </si>
+  <si>
+    <t>Consultar tareas</t>
+  </si>
+  <si>
+    <t>Activar la tarea</t>
+  </si>
+  <si>
+    <t>Activar la tarea en lote</t>
+  </si>
+  <si>
+    <t>Nominar la tarea</t>
+  </si>
+  <si>
+    <t>Nominar tareas en lote</t>
+  </si>
+  <si>
+    <t>Establecer role humano generico</t>
+  </si>
+  <si>
+    <t>Establecer roles humanos generico en lote</t>
+  </si>
+  <si>
+    <t>Crear un callback asíncrono de tarea Lean</t>
+  </si>
+  <si>
+    <t>Registrar la definición de una tarea lean</t>
+  </si>
+  <si>
+    <t>Retirar registro de definición de tarea lean</t>
+  </si>
+  <si>
+    <t>Listar las definiciones de tareas lean</t>
+  </si>
+  <si>
+    <t>Crear una tarea lean</t>
+  </si>
+  <si>
+    <t>Crear una tarea lean asíncrona</t>
+  </si>
+  <si>
+    <t>Operación de salir</t>
+  </si>
+  <si>
+    <t>Operación para saltar</t>
+  </si>
+  <si>
+    <t>Operación de falla</t>
   </si>
 </sst>
 </file>
@@ -740,46 +983,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N82"/>
+  <dimension ref="A1:O82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E82" sqref="E82"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="23" customWidth="1"/>
-    <col min="7" max="11" width="9.140625" style="3"/>
+    <col min="3" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="23" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="83.25" x14ac:dyDescent="0.25">
-      <c r="G1" s="4" t="s">
+    <row r="1" spans="1:15" ht="83.25" x14ac:dyDescent="0.25">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,21 +1033,24 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -812,103 +1058,121 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H9" s="6" t="s">
         <v>12</v>
       </c>
@@ -921,1062 +1185,1284 @@
       <c r="K9" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H13" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H17" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H21" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J24" s="5"/>
-      <c r="K24" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="5"/>
+      <c r="L24" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H25" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" t="s">
         <v>42</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H31" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E33" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="H34" s="6"/>
       <c r="I34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" t="s">
         <v>46</v>
       </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="H35" s="6"/>
       <c r="I35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" t="s">
         <v>47</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J36" s="6"/>
-      <c r="K36" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="6"/>
+      <c r="L36" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" t="s">
         <v>48</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H37" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" t="s">
         <v>49</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H38" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" t="s">
         <v>50</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H39" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" t="s">
         <v>51</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H40" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
         <v>52</v>
       </c>
-      <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="6"/>
+    </row>
+    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" t="s">
         <v>53</v>
       </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="H42" s="6"/>
       <c r="I42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" t="s">
         <v>54</v>
       </c>
-      <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="6"/>
+    </row>
+    <row r="44" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H44" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J44" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="6"/>
+    </row>
+    <row r="46" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
+        <v>142</v>
+      </c>
+      <c r="E46" t="s">
         <v>57</v>
       </c>
-      <c r="G46" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" t="s">
         <v>58</v>
       </c>
-      <c r="G47" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H47" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J47" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" t="s">
         <v>59</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H48" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I48" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J48" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" t="s">
         <v>60</v>
       </c>
-      <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="6"/>
+    </row>
+    <row r="50" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" t="s">
         <v>61</v>
       </c>
-      <c r="G50" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H50" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51" t="s">
         <v>62</v>
       </c>
-      <c r="G51" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H51" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J51" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52" t="s">
         <v>63</v>
       </c>
-      <c r="G52" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H52" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J52" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" t="s">
         <v>64</v>
       </c>
-      <c r="G53" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H53" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J53" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" t="s">
         <v>65</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H54" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J54" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" t="s">
         <v>67</v>
       </c>
-      <c r="G56" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H56" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I56" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J56" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
+        <v>154</v>
+      </c>
+      <c r="E58" t="s">
         <v>69</v>
       </c>
-      <c r="G58" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H58" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J58" s="6"/>
-      <c r="K58" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K58" s="6"/>
+      <c r="L58" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
+        <v>155</v>
+      </c>
+      <c r="E59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
+        <v>156</v>
+      </c>
+      <c r="E60" t="s">
         <v>71</v>
       </c>
-      <c r="G60" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H60" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I60" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J60" s="6"/>
-      <c r="K60" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J60" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K60" s="6"/>
+      <c r="L60" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
+        <v>157</v>
+      </c>
+      <c r="E61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
+        <v>158</v>
+      </c>
+      <c r="E62" t="s">
         <v>73</v>
       </c>
-      <c r="G62" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H62" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I62" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J62" s="6"/>
-      <c r="K62" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K62" s="6"/>
+      <c r="L62" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
+        <v>159</v>
+      </c>
+      <c r="E63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
+        <v>160</v>
+      </c>
+      <c r="E64" t="s">
         <v>75</v>
       </c>
-      <c r="G64" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H64" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I64" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J64" s="6"/>
-      <c r="K64" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J64" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K64" s="6"/>
+      <c r="L64" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
+        <v>161</v>
+      </c>
+      <c r="E65" t="s">
         <v>76</v>
       </c>
-      <c r="G65" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H65" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I65" s="5"/>
+      <c r="I65" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J65" s="5"/>
-      <c r="K65" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="5"/>
+      <c r="L65" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E66" t="s">
         <v>77</v>
       </c>
-      <c r="G66" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H66" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I66" s="5"/>
+      <c r="I66" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J66" s="5"/>
-      <c r="K66" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="5"/>
+      <c r="L66" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
+        <v>163</v>
+      </c>
+      <c r="E67" t="s">
         <v>78</v>
       </c>
-      <c r="G67" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="H67" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I67" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
+        <v>164</v>
+      </c>
+      <c r="E68" t="s">
         <v>79</v>
       </c>
-      <c r="G68" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J68" s="6"/>
-      <c r="K68" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J68" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K68" s="6"/>
+      <c r="L68" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
+        <v>165</v>
+      </c>
+      <c r="E69" t="s">
         <v>80</v>
       </c>
-      <c r="G69" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H69" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I69" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J69" s="6"/>
-      <c r="K69" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J69" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K69" s="6"/>
+      <c r="L69" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
+        <v>166</v>
+      </c>
+      <c r="E70" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
+        <v>167</v>
+      </c>
+      <c r="E71" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
+        <v>168</v>
+      </c>
+      <c r="E72" t="s">
         <v>83</v>
       </c>
-      <c r="G72" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H72" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I72" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J72" s="6"/>
-      <c r="K72" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K72" s="6"/>
+      <c r="L72" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
+        <v>169</v>
+      </c>
+      <c r="E73" t="s">
         <v>84</v>
       </c>
-      <c r="G73" s="6"/>
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
-    </row>
-    <row r="74" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L73" s="6"/>
+    </row>
+    <row r="74" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>85</v>
       </c>
       <c r="D74" t="s">
+        <v>170</v>
+      </c>
+      <c r="E74" t="s">
         <v>86</v>
       </c>
-      <c r="G74" s="6"/>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
-    </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L74" s="6"/>
+    </row>
+    <row r="75" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>87</v>
       </c>
       <c r="D75" t="s">
+        <v>171</v>
+      </c>
+      <c r="E75" t="s">
         <v>88</v>
       </c>
-      <c r="G75" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J75" s="6"/>
+      <c r="H75" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K75" s="6"/>
-    </row>
-    <row r="76" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L75" s="6"/>
+    </row>
+    <row r="76" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
+        <v>172</v>
+      </c>
+      <c r="E76" t="s">
         <v>89</v>
       </c>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="H76" s="6"/>
       <c r="I76" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J76" s="6"/>
+      <c r="J76" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K76" s="6"/>
-    </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L76" s="6"/>
+    </row>
+    <row r="77" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
+        <v>173</v>
+      </c>
+      <c r="E77" t="s">
         <v>90</v>
       </c>
-      <c r="G77" s="6"/>
       <c r="H77" s="6"/>
-      <c r="I77" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K77" s="6"/>
-    </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L77" s="6"/>
+    </row>
+    <row r="78" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
+        <v>174</v>
+      </c>
+      <c r="E78" t="s">
         <v>91</v>
       </c>
-      <c r="G78" s="6"/>
-      <c r="H78" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="H78" s="6"/>
       <c r="I78" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J78" s="6"/>
+      <c r="J78" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K78" s="6"/>
-    </row>
-    <row r="79" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L78" s="6"/>
+    </row>
+    <row r="79" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
+        <v>175</v>
+      </c>
+      <c r="E79" t="s">
         <v>92</v>
       </c>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="H79" s="6"/>
       <c r="I79" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J79" s="6"/>
+      <c r="J79" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K79" s="6"/>
-    </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L79" s="6"/>
+    </row>
+    <row r="80" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>93</v>
       </c>
       <c r="D80" t="s">
+        <v>176</v>
+      </c>
+      <c r="E80" t="s">
         <v>94</v>
       </c>
-      <c r="G80" s="6"/>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="L80" s="6"/>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>95</v>
       </c>
       <c r="D81" t="s">
+        <v>177</v>
+      </c>
+      <c r="E81" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
+        <v>178</v>
+      </c>
+      <c r="E82" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clasficacion de las operaciones de los servicios SOA
</commit_message>
<xml_diff>
--- a/Analisis/Portafolio_Servicios_SOA.xlsx
+++ b/Analisis/Portafolio_Servicios_SOA.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="PORTAFOLIO_SERVICIOS" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PORTAFOLIO_SERVICIOS!$A$2:$P$82</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -430,9 +433,6 @@
     <t>Liberar tareas en lote</t>
   </si>
   <si>
-    <t>Remover tarea</t>
-  </si>
-  <si>
     <t>Re-iniciar la tarea</t>
   </si>
   <si>
@@ -550,7 +550,25 @@
     <t>Operación de falla</t>
   </si>
   <si>
-    <t>Remover tarea en lote</t>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>ADMINISTRATIVA</t>
+  </si>
+  <si>
+    <t>TASKLIST CLIENT</t>
+  </si>
+  <si>
+    <t>HUMANTASK PROCESSOR</t>
+  </si>
+  <si>
+    <t>PARTICIPANT EXECUTED</t>
+  </si>
+  <si>
+    <t>Remover la notificación</t>
+  </si>
+  <si>
+    <t>Remover notificaciones en lote</t>
   </si>
 </sst>
 </file>
@@ -986,13 +1004,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F67" sqref="F67"/>
+      <selection pane="bottomRight" activeCell="N73" sqref="N73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,10 +1020,11 @@
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="23" customWidth="1"/>
     <col min="9" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="83.25" x14ac:dyDescent="0.25">
@@ -1023,7 +1043,6 @@
       <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
@@ -1057,8 +1076,11 @@
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N2" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -1087,8 +1109,11 @@
       <c r="M3" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N3" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D4" s="3">
         <v>2</v>
       </c>
@@ -1111,8 +1136,11 @@
       <c r="M4" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N4" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D5" s="3">
         <v>3</v>
       </c>
@@ -1135,8 +1163,11 @@
       <c r="M5" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N5" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D6" s="3">
         <v>4</v>
       </c>
@@ -1151,8 +1182,11 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N6" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D7" s="3">
         <v>5</v>
       </c>
@@ -1175,8 +1209,11 @@
       <c r="M7" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N7" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D8" s="3">
         <v>6</v>
       </c>
@@ -1191,8 +1228,11 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N8" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D9" s="3">
         <v>7</v>
       </c>
@@ -1217,8 +1257,11 @@
       <c r="M9" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N9" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D10" s="3">
         <v>8</v>
       </c>
@@ -1233,8 +1276,11 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N10" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D11" s="3">
         <v>9</v>
       </c>
@@ -1257,8 +1303,11 @@
       <c r="M11" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N11" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D12" s="3">
         <v>10</v>
       </c>
@@ -1281,8 +1330,11 @@
       <c r="M12" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D13" s="3">
         <v>11</v>
       </c>
@@ -1305,8 +1357,11 @@
       <c r="M13" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D14" s="3">
         <v>12</v>
       </c>
@@ -1329,8 +1384,11 @@
       <c r="M14" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N14" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D15" s="3">
         <v>13</v>
       </c>
@@ -1353,8 +1411,11 @@
       <c r="M15" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="D16" s="3">
         <v>14</v>
       </c>
@@ -1369,8 +1430,11 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D17" s="3">
         <v>15</v>
       </c>
@@ -1393,8 +1457,11 @@
       <c r="M17" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D18" s="3">
         <v>16</v>
       </c>
@@ -1409,8 +1476,11 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D19" s="3">
         <v>17</v>
       </c>
@@ -1433,8 +1503,11 @@
       <c r="M19" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D20" s="3">
         <v>18</v>
       </c>
@@ -1457,8 +1530,11 @@
       <c r="M20" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3">
         <v>19</v>
       </c>
@@ -1481,8 +1557,11 @@
       <c r="M21" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D22" s="3">
         <v>20</v>
       </c>
@@ -1505,8 +1584,11 @@
       <c r="M22" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D23" s="3">
         <v>21</v>
       </c>
@@ -1529,8 +1611,11 @@
       <c r="M23" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D24" s="3">
         <v>22</v>
       </c>
@@ -1549,8 +1634,11 @@
       <c r="M24" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D25" s="3">
         <v>23</v>
       </c>
@@ -1573,8 +1661,11 @@
       <c r="M25" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D26" s="3">
         <v>24</v>
       </c>
@@ -1597,8 +1688,11 @@
       <c r="M26" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D27" s="3">
         <v>25</v>
       </c>
@@ -1621,8 +1715,11 @@
       <c r="M27" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D28" s="3">
         <v>26</v>
       </c>
@@ -1639,8 +1736,11 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-    </row>
-    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D29" s="3">
         <v>27</v>
       </c>
@@ -1657,8 +1757,11 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
-    </row>
-    <row r="30" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D30" s="3">
         <v>28</v>
       </c>
@@ -1681,8 +1784,11 @@
       <c r="M30" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D31" s="3">
         <v>29</v>
       </c>
@@ -1705,8 +1811,11 @@
       <c r="M31" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D32" s="3">
         <v>30</v>
       </c>
@@ -1723,8 +1832,11 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D33" s="3">
         <v>31</v>
       </c>
@@ -1741,8 +1853,11 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D34" s="3">
         <v>32</v>
       </c>
@@ -1763,8 +1878,11 @@
       <c r="M34" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D35" s="3">
         <v>33</v>
       </c>
@@ -1785,8 +1903,11 @@
       <c r="M35" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D36" s="3">
         <v>34</v>
       </c>
@@ -1805,8 +1926,11 @@
       <c r="M36" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D37" s="3">
         <v>35</v>
       </c>
@@ -1829,8 +1953,11 @@
       <c r="M37" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D38" s="3">
         <v>36</v>
       </c>
@@ -1853,8 +1980,11 @@
       <c r="M38" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D39" s="3">
         <v>37</v>
       </c>
@@ -1877,8 +2007,11 @@
       <c r="M39" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D40" s="3">
         <v>38</v>
       </c>
@@ -1901,8 +2034,11 @@
       <c r="M40" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D41" s="3">
         <v>39</v>
       </c>
@@ -1917,13 +2053,16 @@
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
-    </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D42" s="3">
         <v>40</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="F42" t="s">
         <v>53</v>
@@ -1939,13 +2078,16 @@
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D43" s="3">
         <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F43" t="s">
         <v>54</v>
@@ -1955,13 +2097,16 @@
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D44" s="3">
         <v>42</v>
       </c>
       <c r="E44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F44" t="s">
         <v>55</v>
@@ -1979,13 +2124,16 @@
       <c r="M44" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D45" s="3">
         <v>43</v>
       </c>
       <c r="E45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F45" t="s">
         <v>56</v>
@@ -1995,13 +2143,16 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N45" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D46" s="3">
         <v>44</v>
       </c>
       <c r="E46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F46" t="s">
         <v>57</v>
@@ -2019,13 +2170,16 @@
       <c r="M46" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D47" s="3">
         <v>45</v>
       </c>
       <c r="E47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F47" t="s">
         <v>58</v>
@@ -2043,13 +2197,16 @@
       <c r="M47" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N47" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D48" s="3">
         <v>46</v>
       </c>
       <c r="E48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F48" t="s">
         <v>59</v>
@@ -2067,13 +2224,16 @@
       <c r="M48" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D49" s="3">
         <v>47</v>
       </c>
       <c r="E49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F49" t="s">
         <v>60</v>
@@ -2083,13 +2243,16 @@
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
-    </row>
-    <row r="50" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N49" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D50" s="3">
         <v>48</v>
       </c>
       <c r="E50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F50" t="s">
         <v>61</v>
@@ -2107,13 +2270,16 @@
       <c r="M50" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N50" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D51" s="3">
         <v>49</v>
       </c>
       <c r="E51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F51" t="s">
         <v>62</v>
@@ -2131,13 +2297,16 @@
       <c r="M51" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N51" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D52" s="3">
         <v>50</v>
       </c>
       <c r="E52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F52" t="s">
         <v>63</v>
@@ -2155,13 +2324,16 @@
       <c r="M52" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N52" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D53" s="3">
         <v>51</v>
       </c>
       <c r="E53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F53" t="s">
         <v>64</v>
@@ -2179,13 +2351,16 @@
       <c r="M53" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N53" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D54" s="3">
         <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F54" t="s">
         <v>65</v>
@@ -2203,24 +2378,30 @@
       <c r="M54" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N54" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D55" s="3">
         <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F55" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N55" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D56" s="3">
         <v>54</v>
       </c>
       <c r="E56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F56" t="s">
         <v>67</v>
@@ -2238,24 +2419,30 @@
       <c r="M56" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N56" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D57" s="3">
         <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F57" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N57" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D58" s="3">
         <v>56</v>
       </c>
       <c r="E58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F58" t="s">
         <v>69</v>
@@ -2273,24 +2460,30 @@
       <c r="M58" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N58" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D59" s="3">
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F59" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="60" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N59" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D60" s="3">
         <v>58</v>
       </c>
       <c r="E60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F60" t="s">
         <v>71</v>
@@ -2308,24 +2501,30 @@
       <c r="M60" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N60" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D61" s="3">
         <v>59</v>
       </c>
       <c r="E61" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F61" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="62" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N61" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D62" s="3">
         <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F62" t="s">
         <v>73</v>
@@ -2343,24 +2542,30 @@
       <c r="M62" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N62" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D63" s="3">
         <v>61</v>
       </c>
       <c r="E63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F63" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="64" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="N63" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" spans="4:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D64" s="3">
         <v>62</v>
       </c>
       <c r="E64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F64" t="s">
         <v>75</v>
@@ -2378,13 +2583,16 @@
       <c r="M64" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N64" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D65" s="3">
         <v>63</v>
       </c>
       <c r="E65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F65" t="s">
         <v>76</v>
@@ -2400,13 +2608,16 @@
       <c r="M65" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N65" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D66" s="3">
         <v>64</v>
       </c>
       <c r="E66" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F66" t="s">
         <v>77</v>
@@ -2422,13 +2633,16 @@
       <c r="M66" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N66" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D67" s="3">
         <v>65</v>
       </c>
       <c r="E67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F67" t="s">
         <v>78</v>
@@ -2439,13 +2653,16 @@
       <c r="J67" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N67" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D68" s="3">
         <v>66</v>
       </c>
       <c r="E68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F68" t="s">
         <v>79</v>
@@ -2463,13 +2680,16 @@
       <c r="M68" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N68" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D69" s="3">
         <v>67</v>
       </c>
       <c r="E69" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F69" t="s">
         <v>80</v>
@@ -2487,35 +2707,44 @@
       <c r="M69" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N69" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="70" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D70" s="3">
         <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F70" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="71" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N70" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D71" s="3">
         <v>69</v>
       </c>
       <c r="E71" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F71" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="72" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N71" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D72" s="3">
         <v>70</v>
       </c>
       <c r="E72" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F72" t="s">
         <v>83</v>
@@ -2533,13 +2762,16 @@
       <c r="M72" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N72" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="73" spans="3:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D73" s="3">
         <v>71</v>
       </c>
       <c r="E73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F73" t="s">
         <v>84</v>
@@ -2549,13 +2781,16 @@
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
       <c r="M73" s="6"/>
-    </row>
-    <row r="74" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="N73" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="74" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>85</v>
       </c>
       <c r="E74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F74" t="s">
         <v>86</v>
@@ -2566,12 +2801,12 @@
       <c r="L74" s="6"/>
       <c r="M74" s="6"/>
     </row>
-    <row r="75" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>87</v>
       </c>
       <c r="E75" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F75" t="s">
         <v>88</v>
@@ -2586,9 +2821,9 @@
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
     </row>
-    <row r="76" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F76" t="s">
         <v>89</v>
@@ -2603,9 +2838,9 @@
       <c r="L76" s="6"/>
       <c r="M76" s="6"/>
     </row>
-    <row r="77" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F77" t="s">
         <v>90</v>
@@ -2618,9 +2853,9 @@
       <c r="L77" s="6"/>
       <c r="M77" s="6"/>
     </row>
-    <row r="78" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F78" t="s">
         <v>91</v>
@@ -2635,9 +2870,9 @@
       <c r="L78" s="6"/>
       <c r="M78" s="6"/>
     </row>
-    <row r="79" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F79" t="s">
         <v>92</v>
@@ -2652,12 +2887,12 @@
       <c r="L79" s="6"/>
       <c r="M79" s="6"/>
     </row>
-    <row r="80" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>93</v>
       </c>
       <c r="E80" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F80" t="s">
         <v>94</v>
@@ -2673,7 +2908,7 @@
         <v>95</v>
       </c>
       <c r="E81" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F81" t="s">
         <v>96</v>
@@ -2681,13 +2916,18 @@
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F82" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:P82">
+    <filterColumn colId="13">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>